<commit_message>
The release FW for 7.0.3.
- Tweeter gain +15dB
- Role back the BT power on/off state which marked
- Modify the press duration to the BT module. This also need to apply into BT module.
- Remove the audio cue delay for play tone correctly. Need to keep watching if any errors.
- Marked the amp mute before setting the amp. Which should be used for TAS_5760.
- Adjust the default audio cue voulme for V3.
- Update the release note and the BT FW for V3.
</commit_message>
<xml_diff>
--- a/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
+++ b/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\on_working_project_code\Hendrix_github\Hendrix_M_Lite_GD\sw\project_files\Hendrix_M\Release\Hendrix_LiteV3_Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\on_working_project_code\Hendrix_M_Lite_GD_nick\sw\project_files\Hendrix_M\Release\Hendrix_LiteV3_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>HDMI</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Release to resolve the issues in 7.0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zound_Hendrix_M_Lite_V3_hwEVT_btswv7.0.3_20220331</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BT output gain correct. Tone play flow corrected.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -895,7 +907,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.399999999999999" x14ac:dyDescent="0.25"/>
@@ -906,7 +918,7 @@
     <col min="4" max="4" width="57.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="9" style="1"/>
     <col min="10" max="10" width="11.25" style="1" customWidth="1"/>
-    <col min="11" max="11" width="34.75" style="5" customWidth="1"/>
+    <col min="11" max="11" width="47.625" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1396,17 +1408,35 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="6">
+        <v>44651</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="G18" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3.1</v>
+      </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="7"/>
+      <c r="J18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -1594,6 +1624,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="72de59d5-254d-430a-8862-e2bf58cab753">6TCUH2D2FU37-209-14454</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72de59d5-254d-430a-8862-e2bf58cab753">
+      <Url>http://intranet.tymphany.com/Departments/sw/_layouts/15/DocIdRedir.aspx?ID=6TCUH2D2FU37-209-14454</Url>
+      <Description>6TCUH2D2FU37-209-14454</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1641,27 +1692,6 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="72de59d5-254d-430a-8862-e2bf58cab753">6TCUH2D2FU37-209-14454</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72de59d5-254d-430a-8862-e2bf58cab753">
-      <Url>http://intranet.tymphany.com/Departments/sw/_layouts/15/DocIdRedir.aspx?ID=6TCUH2D2FU37-209-14454</Url>
-      <Description>6TCUH2D2FU37-209-14454</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1810,9 +1840,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC868924-2FB4-4B6E-A7E3-A0A4F09EF3D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B7F1-42EF-4214-B878-B6DFF3AEC870}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="72de59d5-254d-430a-8862-e2bf58cab753"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1826,17 +1864,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B7F1-42EF-4214-B878-B6DFF3AEC870}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC868924-2FB4-4B6E-A7E3-A0A4F09EF3D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="72de59d5-254d-430a-8862-e2bf58cab753"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Restore to have the reset pin control of the BT module. This resolve the HW reset without clear PDL issue. Set the audio cue play delay to 0ms. With new BT module, the delay will corrupt the audio cue.
This is the release code base of 7.0.4.
</commit_message>
<xml_diff>
--- a/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
+++ b/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>HDMI</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>BT output gain correct. Tone play flow corrected.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.0.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zound_Hendrix_M_Lite_V3_hwEVT_btswv7.0.4_20220415</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resolve the recoonection issues.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1439,17 +1451,35 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="6">
+        <v>44666</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="G19" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3.1</v>
+      </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="7"/>
+      <c r="J19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -1624,27 +1654,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="72de59d5-254d-430a-8862-e2bf58cab753">6TCUH2D2FU37-209-14454</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72de59d5-254d-430a-8862-e2bf58cab753">
-      <Url>http://intranet.tymphany.com/Departments/sw/_layouts/15/DocIdRedir.aspx?ID=6TCUH2D2FU37-209-14454</Url>
-      <Description>6TCUH2D2FU37-209-14454</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1692,6 +1701,27 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="72de59d5-254d-430a-8862-e2bf58cab753">6TCUH2D2FU37-209-14454</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72de59d5-254d-430a-8862-e2bf58cab753">
+      <Url>http://intranet.tymphany.com/Departments/sw/_layouts/15/DocIdRedir.aspx?ID=6TCUH2D2FU37-209-14454</Url>
+      <Description>6TCUH2D2FU37-209-14454</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1840,17 +1870,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B7F1-42EF-4214-B878-B6DFF3AEC870}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC868924-2FB4-4B6E-A7E3-A0A4F09EF3D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="72de59d5-254d-430a-8862-e2bf58cab753"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1864,9 +1886,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC868924-2FB4-4B6E-A7E3-A0A4F09EF3D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B7F1-42EF-4214-B878-B6DFF3AEC870}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="72de59d5-254d-430a-8862-e2bf58cab753"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Remove the workaround of playing charging cue. If A2DP not playing, set default volume for playing AG2 connected tone. FW version ++ for release.
</commit_message>
<xml_diff>
--- a/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
+++ b/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\on_working_project_code\Hendrix_M_Lite_GD_nick\sw\project_files\Hendrix_M\Release\Hendrix_LiteV3_Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working_project_code\Hendrix_M_Lite_GD_nick\sw\project_files\Hendrix_M\Release\Hendrix_LiteV3_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
   <si>
     <t>HDMI</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,26 @@
   </si>
   <si>
     <t>Resolve the recoonection issues.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zound_Hendrix_M_Lite_V3_hwEVT_btswv7.0.5_20220429</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resolve the multi point recoonection issues. Audio cue related issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.0.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zound_Hendrix_M_Lite_V3_hwEVT_btswv7.0.6_20220513</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -919,7 +939,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.399999999999999" x14ac:dyDescent="0.25"/>
@@ -930,7 +950,7 @@
     <col min="4" max="4" width="57.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="9" style="1"/>
     <col min="10" max="10" width="11.25" style="1" customWidth="1"/>
-    <col min="11" max="11" width="47.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.5" style="5" customWidth="1"/>
     <col min="12" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1482,29 +1502,63 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="6">
+        <v>44680</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="G20" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3.1</v>
+      </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="7"/>
+      <c r="J20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="6">
+        <v>44680</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="G21" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3.1</v>
+      </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="J21" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1654,6 +1708,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="72de59d5-254d-430a-8862-e2bf58cab753">6TCUH2D2FU37-209-14454</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72de59d5-254d-430a-8862-e2bf58cab753">
+      <Url>http://intranet.tymphany.com/Departments/sw/_layouts/15/DocIdRedir.aspx?ID=6TCUH2D2FU37-209-14454</Url>
+      <Description>6TCUH2D2FU37-209-14454</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1701,27 +1776,6 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="72de59d5-254d-430a-8862-e2bf58cab753">6TCUH2D2FU37-209-14454</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72de59d5-254d-430a-8862-e2bf58cab753">
-      <Url>http://intranet.tymphany.com/Departments/sw/_layouts/15/DocIdRedir.aspx?ID=6TCUH2D2FU37-209-14454</Url>
-      <Description>6TCUH2D2FU37-209-14454</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1870,9 +1924,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC868924-2FB4-4B6E-A7E3-A0A4F09EF3D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B7F1-42EF-4214-B878-B6DFF3AEC870}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="72de59d5-254d-430a-8862-e2bf58cab753"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1886,17 +1948,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B7F1-42EF-4214-B878-B6DFF3AEC870}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC868924-2FB4-4B6E-A7E3-A0A4F09EF3D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="72de59d5-254d-430a-8862-e2bf58cab753"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
1. Lower the tick of LED server to 37ms to lower the priority 2. Resolve the ZSR-31 issue. Wake up without audio or cannot control the knob, cannot detect the ADC level. This modification restore the feature to resolve the BRH-11.
</commit_message>
<xml_diff>
--- a/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
+++ b/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>HDMI</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -210,6 +210,22 @@
   </si>
   <si>
     <t>Zound_Hendrix_M_Lite_V3_hwEVT_btswv7.0.6_20220513</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Improve the reconnection and audio cue related issues.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.0.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zound_Hendrix_M_Lite_V3_hwEVT_btswv7.0.7_20220513</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resolve the BRH-11. Modify AVCTP to V1.4.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -939,7 +955,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1556,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="6">
-        <v>44680</v>
+        <v>44694</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>45</v>
@@ -1559,20 +1575,40 @@
       <c r="J21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K21" s="7"/>
+      <c r="K21" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="6">
+        <v>44699</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="G22" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3.1</v>
+      </c>
       <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="7"/>
+      <c r="J22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1708,27 +1744,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="72de59d5-254d-430a-8862-e2bf58cab753">6TCUH2D2FU37-209-14454</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72de59d5-254d-430a-8862-e2bf58cab753">
-      <Url>http://intranet.tymphany.com/Departments/sw/_layouts/15/DocIdRedir.aspx?ID=6TCUH2D2FU37-209-14454</Url>
-      <Description>6TCUH2D2FU37-209-14454</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1776,6 +1791,27 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="72de59d5-254d-430a-8862-e2bf58cab753">6TCUH2D2FU37-209-14454</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72de59d5-254d-430a-8862-e2bf58cab753">
+      <Url>http://intranet.tymphany.com/Departments/sw/_layouts/15/DocIdRedir.aspx?ID=6TCUH2D2FU37-209-14454</Url>
+      <Description>6TCUH2D2FU37-209-14454</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1924,17 +1960,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B7F1-42EF-4214-B878-B6DFF3AEC870}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC868924-2FB4-4B6E-A7E3-A0A4F09EF3D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="72de59d5-254d-430a-8862-e2bf58cab753"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1948,9 +1976,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC868924-2FB4-4B6E-A7E3-A0A4F09EF3D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F69B7F1-42EF-4214-B878-B6DFF3AEC870}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="72de59d5-254d-430a-8862-e2bf58cab753"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Modify the tweeter AMP output PWM to 768K to resolve the power consumption issue.
</commit_message>
<xml_diff>
--- a/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
+++ b/sw/project_files/Hendrix_M/Release/Hendrix_LiteV3_Notes/RD-Release history.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
   <si>
     <t>HDMI</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -258,6 +258,22 @@
   </si>
   <si>
     <t>To resolve BRH-36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V3 MP Firmware</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zound_Hendrix_M_Lite_V3_hwEVT_btswv7.1.0_20220718</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modify the amp RT9120S output PWM to 768KHz to lower the power consumption.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -987,7 +1003,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1735,18 +1751,36 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+    <row r="26" spans="1:11" ht="32.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="6">
+        <v>44760</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="G26" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3.1</v>
+      </c>
       <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="7"/>
+      <c r="J26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>

</xml_diff>